<commit_message>
STU_MTCUXC: Llenado de la matriz
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_MTCUXC.xlsx
+++ b/STU/Analisis y Diseño/STU_MTCUXC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jramirezh2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\projects\RPJA\STU\Analisis y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>CUS01: Busqueda de vehiculos</t>
   </si>
@@ -53,16 +53,22 @@
     <t>Clases</t>
   </si>
   <si>
-    <t>CLS1:</t>
-  </si>
-  <si>
-    <t>CLS2:</t>
-  </si>
-  <si>
-    <t>CLS3:</t>
-  </si>
-  <si>
-    <t>CLS4:</t>
+    <t>CLS1: Vehiculo</t>
+  </si>
+  <si>
+    <t>CLS2: Comentario</t>
+  </si>
+  <si>
+    <t>CLS3: Denuncia</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>CLS4: Propietario</t>
+  </si>
+  <si>
+    <t>CLS5: Infraccion</t>
   </si>
 </sst>
 </file>
@@ -395,18 +401,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
@@ -415,7 +426,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -429,43 +440,109 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>